<commit_message>
Bugfix in Edge Weighting Script
</commit_message>
<xml_diff>
--- a/01_BachelorWifoMannheim/04_Graph/CourseSkillWeights_Bachelor.xlsx
+++ b/01_BachelorWifoMannheim/04_Graph/CourseSkillWeights_Bachelor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailunimannheimde-my.sharepoint.com/personal/pstapf_mail_uni-mannheim_de/Documents/Uni/Master/Masterarbeit/Course_Suggestion/01_BachelorWifoMannheim/04_Graph/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_68BDB2A7D33057014B5A3E11595ED87656CDC4D6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{466625FD-16E1-4C5B-A1B2-8089EC84EF60}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_68BDB2A7D33057014B5A3E11595ED87656CDC4D6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91BDD388-3A03-417C-AFEF-27A17867EA80}"/>
   <bookViews>
-    <workbookView xWindow="-25245" yWindow="1215" windowWidth="21600" windowHeight="14070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -624,7 +624,7 @@
   <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A91"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -663,7 +663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -680,7 +680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.1</v>
       </c>
@@ -935,7 +935,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>109.86022943911171</v>
       </c>
@@ -952,7 +952,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>98.123797263861775</v>
       </c>
@@ -969,7 +969,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>73.336338915550499</v>
       </c>
@@ -986,7 +986,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>82.817125619478531</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0.1</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>2776</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.1</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0.1</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0.1</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0.1</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>1776</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0.1</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0.1</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0.1</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0.1</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>5332</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0.1</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0.1</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0.1</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0.1</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0.1</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0.1</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0.1</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0.1</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0.1</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0.1</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0.1</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0.1</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>0.1</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0.1</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0.1</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0.1</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>0.1</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0.1</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0.1</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0.1</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>2676</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0.1</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>0.1</v>
       </c>
@@ -2178,9 +2178,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E91" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
+    <filterColumn colId="1">
       <filters>
-        <filter val="0,001"/>
+        <filter val="CS 302 Praktische Informatik I Practical Computer Science I"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>